<commit_message>
Forgot to make a dev branch, worked before this commit
</commit_message>
<xml_diff>
--- a/Revit-NTR-Exporter/NTR_CONFIG.xlsx
+++ b/Revit-NTR-Exporter/NTR_CONFIG.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Revit-PCF-Exporter\Revit-NTR-Exporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Revit-PCF-Exporter\Revit-NTR-Exporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
     <sheet name="AUFT" sheetId="5" r:id="rId2"/>
     <sheet name="TEXT" sheetId="4" r:id="rId3"/>
+    <sheet name="LAST" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>TMONT</t>
   </si>
@@ -53,6 +54,39 @@
   </si>
   <si>
     <t>Two</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>TRANS</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>GAMMED</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>DISTR</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>90</t>
   </si>
 </sst>
 </file>
@@ -407,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -506,4 +540,79 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <picture r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First draft of writing configuration data from excel
</commit_message>
<xml_diff>
--- a/Revit-NTR-Exporter/NTR_CONFIG.xlsx
+++ b/Revit-NTR-Exporter/NTR_CONFIG.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
     <sheet name="AUFT" sheetId="5" r:id="rId2"/>
     <sheet name="TEXT" sheetId="4" r:id="rId3"/>
     <sheet name="LAST" sheetId="7" r:id="rId4"/>
+    <sheet name="DN" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="47">
   <si>
     <t>TMONT</t>
   </si>
@@ -87,6 +88,87 @@
   </si>
   <si>
     <t>90</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>ISOTYP</t>
+  </si>
+  <si>
+    <t>ISODICKE</t>
+  </si>
+  <si>
+    <t>NORM</t>
+  </si>
+  <si>
+    <t>ISOLERING</t>
+  </si>
+  <si>
+    <t>EN 10216-2'</t>
+  </si>
+  <si>
+    <t>DN10</t>
+  </si>
+  <si>
+    <t>DN15</t>
+  </si>
+  <si>
+    <t>DN20</t>
+  </si>
+  <si>
+    <t>DN25</t>
+  </si>
+  <si>
+    <t>DN32</t>
+  </si>
+  <si>
+    <t>DN40</t>
+  </si>
+  <si>
+    <t>DN50</t>
+  </si>
+  <si>
+    <t>DN65</t>
+  </si>
+  <si>
+    <t>DN80</t>
+  </si>
+  <si>
+    <t>DN100</t>
+  </si>
+  <si>
+    <t>DN125</t>
+  </si>
+  <si>
+    <t>DN150</t>
+  </si>
+  <si>
+    <t>DN200</t>
+  </si>
+  <si>
+    <t>DN250</t>
+  </si>
+  <si>
+    <t>DN300</t>
+  </si>
+  <si>
+    <t>DN350</t>
+  </si>
+  <si>
+    <t>DN400</t>
+  </si>
+  <si>
+    <t>DN450</t>
+  </si>
+  <si>
+    <t>DN500</t>
+  </si>
+  <si>
+    <t>DN600</t>
   </si>
 </sst>
 </file>
@@ -122,9 +204,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,7 +525,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +566,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +595,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,9 +629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -615,4 +696,823 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <picture r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1">
+        <v>110</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>21.3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1">
+        <v>110</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1">
+        <v>26.9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1">
+        <v>110</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1">
+        <v>110</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42.4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1">
+        <v>110</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1">
+        <v>48.3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1">
+        <v>110</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1">
+        <v>60.3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1">
+        <v>110</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="1">
+        <v>110</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1">
+        <v>88.9</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="1">
+        <v>110</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1">
+        <v>114.3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="1">
+        <v>110</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1">
+        <v>110</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1">
+        <v>168.3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="1">
+        <v>110</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="1">
+        <v>219.1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="1">
+        <v>110</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1">
+        <v>273</v>
+      </c>
+      <c r="C28" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="1">
+        <v>110</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1">
+        <v>323.89999999999998</v>
+      </c>
+      <c r="C30" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="1">
+        <v>110</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="1">
+        <v>355.6</v>
+      </c>
+      <c r="C32" s="1">
+        <v>8</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="1">
+        <v>110</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="1">
+        <v>406.4</v>
+      </c>
+      <c r="C34" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="1">
+        <v>110</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="1">
+        <v>457</v>
+      </c>
+      <c r="C36" s="1">
+        <v>10</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="1">
+        <v>110</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="1">
+        <v>508</v>
+      </c>
+      <c r="C38" s="1">
+        <v>11</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="1">
+        <v>110</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="1">
+        <v>610</v>
+      </c>
+      <c r="C40" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="1">
+        <v>110</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Forgot to save excel
</commit_message>
<xml_diff>
--- a/Revit-NTR-Exporter/NTR_CONFIG.xlsx
+++ b/Revit-NTR-Exporter/NTR_CONFIG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="TEXT" sheetId="4" r:id="rId3"/>
     <sheet name="LAST" sheetId="7" r:id="rId4"/>
     <sheet name="DN" sheetId="9" r:id="rId5"/>
+    <sheet name="IS" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="53">
   <si>
     <t>TMONT</t>
   </si>
@@ -169,6 +170,24 @@
   </si>
   <si>
     <t>DN600</t>
+  </si>
+  <si>
+    <t>GAM</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>DICKEBL</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>GAMBL</t>
+  </si>
+  <si>
+    <t>2700</t>
   </si>
 </sst>
 </file>
@@ -702,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1515,4 +1534,51 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <picture r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented DN writer and other small things
</commit_message>
<xml_diff>
--- a/Revit-NTR-Exporter/NTR_CONFIG.xlsx
+++ b/Revit-NTR-Exporter/NTR_CONFIG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="80">
   <si>
     <t>TMONT</t>
   </si>
@@ -49,15 +49,6 @@
     <t>TEXT</t>
   </si>
   <si>
-    <t>MyProject</t>
-  </si>
-  <si>
-    <t>One</t>
-  </si>
-  <si>
-    <t>Two</t>
-  </si>
-  <si>
     <t>NAME</t>
   </si>
   <si>
@@ -109,9 +100,6 @@
     <t>ISOLERING</t>
   </si>
   <si>
-    <t>EN 10216-2'</t>
-  </si>
-  <si>
     <t>DN10</t>
   </si>
   <si>
@@ -188,6 +176,99 @@
   </si>
   <si>
     <t>2700</t>
+  </si>
+  <si>
+    <t>'EN 10216-2'</t>
+  </si>
+  <si>
+    <t>17.2</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>21.3</t>
+  </si>
+  <si>
+    <t>26.9</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>33.7</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>42.4</t>
+  </si>
+  <si>
+    <t>48.3</t>
+  </si>
+  <si>
+    <t>60.3</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>76.1</t>
+  </si>
+  <si>
+    <t>88.9</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>114.3</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>139.7</t>
+  </si>
+  <si>
+    <t>168.3</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>219.1</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>323.9</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>355.6</t>
+  </si>
+  <si>
+    <t>406.4</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>'MyProject'</t>
+  </si>
+  <si>
+    <t>'One'</t>
+  </si>
+  <si>
+    <t>'Two'</t>
   </si>
 </sst>
 </file>
@@ -223,10 +304,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +628,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +669,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,8 +683,8 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
+      <c r="A2" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -614,12 +698,14 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.28515625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -631,11 +717,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +734,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -657,58 +745,58 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -721,718 +809,720 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="1">
-        <v>17.2</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.8</v>
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1">
         <v>110</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1">
-        <v>21.3</v>
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1">
         <v>110</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1">
-        <v>26.9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.2999999999999998</v>
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1">
         <v>110</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="1">
-        <v>33.700000000000003</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2.6</v>
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1">
         <v>110</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="1">
-        <v>42.4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2.6</v>
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1">
         <v>110</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="1">
-        <v>48.3</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2.6</v>
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1">
         <v>110</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1">
-        <v>60.3</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2.9</v>
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1">
         <v>110</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="1">
-        <v>76.099999999999994</v>
-      </c>
-      <c r="C16" s="1">
-        <v>2.9</v>
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E16" s="1">
         <v>110</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1">
-        <v>88.9</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3.2</v>
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E18" s="1">
         <v>110</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="1">
-        <v>114.3</v>
-      </c>
-      <c r="C20" s="1">
-        <v>3.6</v>
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1">
         <v>110</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="1">
-        <v>139.69999999999999</v>
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C22" s="1">
         <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E22" s="1">
         <v>110</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="1">
-        <v>168.3</v>
-      </c>
-      <c r="C24" s="1">
-        <v>4.5</v>
+        <v>34</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E24" s="1">
         <v>110</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="1">
-        <v>219.1</v>
-      </c>
-      <c r="C26" s="1">
-        <v>6.3</v>
+        <v>35</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E26" s="1">
         <v>110</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1">
         <v>273</v>
       </c>
-      <c r="C28" s="1">
-        <v>6.3</v>
+      <c r="C28" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E28" s="1">
         <v>110</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="1">
-        <v>323.89999999999998</v>
-      </c>
-      <c r="C30" s="1">
-        <v>7.1</v>
+        <v>37</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E30" s="1">
         <v>110</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="1">
-        <v>355.6</v>
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C32" s="1">
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E32" s="1">
         <v>110</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="1">
-        <v>406.4</v>
-      </c>
-      <c r="C34" s="1">
-        <v>8.8000000000000007</v>
+        <v>39</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E34" s="1">
         <v>110</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1">
         <v>457</v>
@@ -1441,38 +1531,38 @@
         <v>10</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E36" s="1">
         <v>110</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1">
         <v>508</v>
@@ -1481,53 +1571,53 @@
         <v>11</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E38" s="1">
         <v>110</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1">
         <v>610</v>
       </c>
-      <c r="C40" s="1">
-        <v>12.5</v>
+      <c r="C40" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E40" s="1">
         <v>110</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1540,45 +1630,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <picture r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <picture r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>